<commit_message>
PDF and CDF -v8
</commit_message>
<xml_diff>
--- a/Data Analysis/PoroPermSampleData.xlsx
+++ b/Data Analysis/PoroPermSampleData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE8E2BA-3883-4F33-95EB-EC7ACDA8E202}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540E7DCA-EA93-410A-8E30-1E52B2020068}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     </r>
   </si>
   <si>
-    <t>Permeability (k)</t>
+    <t>Permeability (mD)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>